<commit_message>
new data & update
</commit_message>
<xml_diff>
--- a/COVID_EXCEL/COVID II.xlsx
+++ b/COVID_EXCEL/COVID II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\COVID-19\COVID_EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053725C-9CB6-4C54-9594-094A75CE6E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7429BDFF-F36E-4850-833C-E4BBCC016BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{9D9ED99E-6145-4CB3-89AD-BE6ED8ABD009}"/>
   </bookViews>
@@ -13906,10 +13906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF55AAC-F8AB-4612-B8B4-806DD7153254}">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+      <selection activeCell="F111" sqref="F111:H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16398,11 +16398,11 @@
         <v>44124</v>
       </c>
       <c r="G110">
-        <f>AVERAGE(B110:B116)</f>
+        <f t="shared" ref="G110:H112" si="114">AVERAGE(B110:B116)</f>
         <v>9855.4285714285706</v>
       </c>
       <c r="H110">
-        <f>AVERAGE(C110:C116)</f>
+        <f t="shared" si="114"/>
         <v>65.571428571428569</v>
       </c>
     </row>
@@ -16421,11 +16421,11 @@
         <v>44125</v>
       </c>
       <c r="G111">
-        <f>AVERAGE(B111:B117)</f>
+        <f t="shared" si="114"/>
         <v>10979.285714285714</v>
       </c>
       <c r="H111">
-        <f>AVERAGE(C111:C117)</f>
+        <f t="shared" si="114"/>
         <v>87.571428571428569</v>
       </c>
     </row>
@@ -16444,15 +16444,15 @@
         <v>44126</v>
       </c>
       <c r="G112">
-        <f>AVERAGE(B112:B118)</f>
+        <f t="shared" si="114"/>
         <v>12018.571428571429</v>
       </c>
       <c r="H112">
-        <f>AVERAGE(C112:C118)</f>
+        <f t="shared" si="114"/>
         <v>95.142857142857139</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44121</v>
       </c>
@@ -16462,8 +16462,20 @@
       <c r="C113">
         <v>47</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F113" s="1">
+        <f t="shared" ref="F113:F115" si="115">A119</f>
+        <v>44127</v>
+      </c>
+      <c r="G113">
+        <f t="shared" ref="G113:G115" si="116">AVERAGE(B113:B119)</f>
+        <v>13323.285714285714</v>
+      </c>
+      <c r="H113">
+        <f t="shared" ref="H113:H115" si="117">AVERAGE(C113:C119)</f>
+        <v>100.28571428571429</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44122</v>
       </c>
@@ -16473,8 +16485,20 @@
       <c r="C114">
         <v>69</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F114" s="1">
+        <f t="shared" si="115"/>
+        <v>44128</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="116"/>
+        <v>14568.857142857143</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="117"/>
+        <v>115.14285714285714</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44123</v>
       </c>
@@ -16484,8 +16508,20 @@
       <c r="C115">
         <v>73</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F115" s="1">
+        <f t="shared" si="115"/>
+        <v>44129</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="116"/>
+        <v>15935.714285714286</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="117"/>
+        <v>123.57142857142857</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44124</v>
       </c>
@@ -16496,7 +16532,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44125</v>
       </c>
@@ -16507,7 +16543,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44126</v>
       </c>
@@ -16516,6 +16552,39 @@
       </c>
       <c r="C118">
         <v>136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>44127</v>
+      </c>
+      <c r="B119">
+        <v>19143</v>
+      </c>
+      <c r="C119">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44128</v>
+      </c>
+      <c r="B120">
+        <v>19644</v>
+      </c>
+      <c r="C120">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>44129</v>
+      </c>
+      <c r="B121">
+        <v>21273</v>
+      </c>
+      <c r="C121">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -27752,7 +27821,7 @@
       </c>
       <c r="B115" s="1">
         <f>'REAL DATA'!F113</f>
-        <v>0</v>
+        <v>44127</v>
       </c>
       <c r="C115">
         <f t="shared" si="47"/>
@@ -27776,7 +27845,7 @@
       </c>
       <c r="H115">
         <f>'REAL DATA'!G113</f>
-        <v>0</v>
+        <v>13323.285714285714</v>
       </c>
       <c r="I115">
         <v>9.9999999999997868E-3</v>
@@ -27870,7 +27939,7 @@
       </c>
       <c r="B116" s="1">
         <f>'REAL DATA'!F114</f>
-        <v>0</v>
+        <v>44128</v>
       </c>
       <c r="C116">
         <f t="shared" si="47"/>
@@ -27894,7 +27963,7 @@
       </c>
       <c r="H116">
         <f>'REAL DATA'!G114</f>
-        <v>0</v>
+        <v>14568.857142857143</v>
       </c>
       <c r="I116">
         <v>0</v>
@@ -27988,7 +28057,7 @@
       </c>
       <c r="B117" s="1">
         <f>'REAL DATA'!F115</f>
-        <v>0</v>
+        <v>44129</v>
       </c>
       <c r="C117">
         <f t="shared" si="47"/>
@@ -28012,7 +28081,7 @@
       </c>
       <c r="H117">
         <f>'REAL DATA'!G115</f>
-        <v>0</v>
+        <v>15935.714285714286</v>
       </c>
       <c r="I117">
         <v>0</v>

</xml_diff>